<commit_message>
Documento Historias de Usuario: Modificado 1.0
</commit_message>
<xml_diff>
--- a/Proyecto Final - Historias de Usuario.xlsx
+++ b/Proyecto Final - Historias de Usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Práctica Final Verificación y Validación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D008F2-1DB2-40E5-B3D1-A308D7BE812C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7963DDD7-0648-4FA3-966B-2E402C36A3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>Julen Huarte Liras</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>HU#3 Como integrante del equipo de desarrollo quiero desarrollar clases correspondientes al modelo del proyecto para poder facilitar el desarrollo.</t>
+  </si>
+  <si>
+    <t>HU#2_T7 Aplicar actions en el proyecto.</t>
+  </si>
+  <si>
+    <t>HU#2_T6 Aplicar pre-commit en el proyecto.</t>
   </si>
 </sst>
 </file>
@@ -283,7 +289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -306,11 +312,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -319,6 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -812,196 +830,215 @@
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1" t="s">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+      <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="8"/>
     </row>
     <row r="88" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>

</xml_diff>

<commit_message>
Documento de Historias de Usuario: Modificación 2.0
</commit_message>
<xml_diff>
--- a/Proyecto Final - Historias de Usuario.xlsx
+++ b/Proyecto Final - Historias de Usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Práctica Final Verificación y Validación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7963DDD7-0648-4FA3-966B-2E402C36A3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEDEA4F-640E-41C4-96B5-CD0D7F08D1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,60 +110,6 @@
     <t>HU#2 Como manager del proyecto quiero configurar un entorno de trabajo para desempeñar correctamente las tareas del desarrollo del proyecto.</t>
   </si>
   <si>
-    <t>HU#3 Como desarrollador quiero que el proyecto tenga validación de los parámetros de entrada.</t>
-  </si>
-  <si>
-    <t>HU#3_T1 Creación de los tests correspondientes a la etapa REQUEST.</t>
-  </si>
-  <si>
-    <t>HU#3_T2 Creación de las clases correspondientes a la etapa REQUEST con su correspondiente implementación.</t>
-  </si>
-  <si>
-    <t>HU#4 Como Product Owner quiero que el proyecto disponga de controladores para controlar las comunicaciones entre clases de la etapa REQUEST y las de la etapa SERVICE.</t>
-  </si>
-  <si>
-    <t>HU#4_T1 Creación de los tests correspondientes a la etapa CONTROLLER.</t>
-  </si>
-  <si>
-    <t>HU#4_T2 Creación de las clases correspondientes a la etapa CONTROLLER con su correspondiente implementación.</t>
-  </si>
-  <si>
-    <t>HU#5_T1 Creación de los tests correspondientes a la etapa SERVICE.</t>
-  </si>
-  <si>
-    <t>HU#5_T2 Creación de las clases correspondientes a la etapa SERVICE con su correspondiente implementación.</t>
-  </si>
-  <si>
-    <t>HU#5 Como desarrollador quiero que el proyecto tenga unas clases que provean el servicio e implementen la lógica de negocio.</t>
-  </si>
-  <si>
-    <t>HU#6 Como manager del proyecto quiero que el proyecto disponga de unas interfaces que se encarguen de dar respuesta a las peticiones de la etapa SERVICE.</t>
-  </si>
-  <si>
-    <t>HU#6_T1 Creación de los tests correspondientes a la etapa DATASOURCE.</t>
-  </si>
-  <si>
-    <t>HU#6_T2 Creación de las clases correspondientes a la etapa DATASOURCE con su correspondiente implementación.</t>
-  </si>
-  <si>
-    <t>HU#7 Como Product Owner quiero que el proyecto tenga unas clases para que se encarguen de realizar llamadas a la API y recibir su respuesta con su correspondiente tratamiento.</t>
-  </si>
-  <si>
-    <t>HU#7_T1 Creación de los tests correspondientes a las clases que llamen a la API.</t>
-  </si>
-  <si>
-    <t>HU#7_T2 Creación de las clases que realicen llamadas a la API de coinlore.</t>
-  </si>
-  <si>
-    <t>HU#8 Como Desarrollador quiero que el proyecto almacene los datos obtenidos de la API en caché.</t>
-  </si>
-  <si>
-    <t>HU#8_T1 Creación de los tests correspondientes a las clases que se encarguen del almacenamiento de los datos en caché.</t>
-  </si>
-  <si>
-    <t>HU#8_T2 Creación de las clases que se encarguen del almacenamiento de los datos en caché.</t>
-  </si>
-  <si>
     <t>Julen, Yeray, Luis, Javi</t>
   </si>
   <si>
@@ -213,6 +159,60 @@
   </si>
   <si>
     <t>HU#2_T6 Aplicar pre-commit en el proyecto.</t>
+  </si>
+  <si>
+    <t>HU#4 Como desarrollador quiero que el proyecto tenga validación de los parámetros de entrada.</t>
+  </si>
+  <si>
+    <t>HU#4_T1 Creación de los tests correspondientes a la etapa REQUEST.</t>
+  </si>
+  <si>
+    <t>HU#4_T2 Creación de las clases correspondientes a la etapa REQUEST con su correspondiente implementación.</t>
+  </si>
+  <si>
+    <t>HU#5 Como Product Owner quiero que el proyecto disponga de controladores para controlar las comunicaciones entre clases de la etapa REQUEST y las de la etapa SERVICE.</t>
+  </si>
+  <si>
+    <t>HU#5_T1 Creación de los tests correspondientes a la etapa CONTROLLER.</t>
+  </si>
+  <si>
+    <t>HU#5_T2 Creación de las clases correspondientes a la etapa CONTROLLER con su correspondiente implementación.</t>
+  </si>
+  <si>
+    <t>HU#6 Como desarrollador quiero que el proyecto tenga unas clases que provean el servicio e implementen la lógica de negocio.</t>
+  </si>
+  <si>
+    <t>HU#6_T1 Creación de los tests correspondientes a la etapa SERVICE.</t>
+  </si>
+  <si>
+    <t>HU#6_T2 Creación de las clases correspondientes a la etapa SERVICE con su correspondiente implementación.</t>
+  </si>
+  <si>
+    <t>HU#7 Como manager del proyecto quiero que el proyecto disponga de unas interfaces que se encarguen de dar respuesta a las peticiones de la etapa SERVICE.</t>
+  </si>
+  <si>
+    <t>HU#8_T1 Creación de los tests correspondientes a la etapa DATASOURCE.</t>
+  </si>
+  <si>
+    <t>HU#8_T2 Creación de las clases correspondientes a la etapa DATASOURCE con su correspondiente implementación.</t>
+  </si>
+  <si>
+    <t>HU#9 Como Product Owner quiero que el proyecto tenga unas clases para que se encarguen de realizar llamadas a la API y recibir su respuesta con su correspondiente tratamiento.</t>
+  </si>
+  <si>
+    <t>HU#9_T1 Creación de los tests correspondientes a las clases que llamen a la API.</t>
+  </si>
+  <si>
+    <t>HU#9_T2 Creación de las clases que realicen llamadas a la API de coinlore.</t>
+  </si>
+  <si>
+    <t>HU#10_T1 Creación de los tests correspondientes a las clases que se encarguen del almacenamiento de los datos en caché.</t>
+  </si>
+  <si>
+    <t>HU#10_T2 Creación de las clases que se encarguen del almacenamiento de los datos en caché.</t>
+  </si>
+  <si>
+    <t>HU#10 Como desarrollador quiero que el proyecto almacene los datos obtenidos de la API en caché.</t>
   </si>
 </sst>
 </file>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -711,7 +711,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -723,7 +723,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -732,10 +732,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -744,10 +744,10 @@
         <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -756,10 +756,10 @@
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -776,10 +776,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -791,7 +791,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -800,10 +800,10 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -822,16 +822,16 @@
         <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -839,7 +839,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -847,7 +847,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -855,29 +855,29 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -885,27 +885,27 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -913,27 +913,27 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -941,27 +941,27 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -969,29 +969,29 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -999,7 +999,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="43" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>

</xml_diff>

<commit_message>
Documento de Historias de Usuario: Modificación 3.0
</commit_message>
<xml_diff>
--- a/Proyecto Final - Historias de Usuario.xlsx
+++ b/Proyecto Final - Historias de Usuario.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Práctica Final Verificación y Validación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEDEA4F-640E-41C4-96B5-CD0D7F08D1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11996859-83CD-45C2-BC05-08D8665ABB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
   <si>
     <t>Julen Huarte Liras</t>
   </si>
@@ -161,58 +161,118 @@
     <t>HU#2_T6 Aplicar pre-commit en el proyecto.</t>
   </si>
   <si>
-    <t>HU#4 Como desarrollador quiero que el proyecto tenga validación de los parámetros de entrada.</t>
-  </si>
-  <si>
-    <t>HU#4_T1 Creación de los tests correspondientes a la etapa REQUEST.</t>
-  </si>
-  <si>
-    <t>HU#4_T2 Creación de las clases correspondientes a la etapa REQUEST con su correspondiente implementación.</t>
-  </si>
-  <si>
-    <t>HU#5 Como Product Owner quiero que el proyecto disponga de controladores para controlar las comunicaciones entre clases de la etapa REQUEST y las de la etapa SERVICE.</t>
-  </si>
-  <si>
-    <t>HU#5_T1 Creación de los tests correspondientes a la etapa CONTROLLER.</t>
-  </si>
-  <si>
-    <t>HU#5_T2 Creación de las clases correspondientes a la etapa CONTROLLER con su correspondiente implementación.</t>
-  </si>
-  <si>
-    <t>HU#6 Como desarrollador quiero que el proyecto tenga unas clases que provean el servicio e implementen la lógica de negocio.</t>
-  </si>
-  <si>
-    <t>HU#6_T1 Creación de los tests correspondientes a la etapa SERVICE.</t>
-  </si>
-  <si>
-    <t>HU#6_T2 Creación de las clases correspondientes a la etapa SERVICE con su correspondiente implementación.</t>
-  </si>
-  <si>
-    <t>HU#7 Como manager del proyecto quiero que el proyecto disponga de unas interfaces que se encarguen de dar respuesta a las peticiones de la etapa SERVICE.</t>
-  </si>
-  <si>
-    <t>HU#8_T1 Creación de los tests correspondientes a la etapa DATASOURCE.</t>
-  </si>
-  <si>
-    <t>HU#8_T2 Creación de las clases correspondientes a la etapa DATASOURCE con su correspondiente implementación.</t>
-  </si>
-  <si>
-    <t>HU#9 Como Product Owner quiero que el proyecto tenga unas clases para que se encarguen de realizar llamadas a la API y recibir su respuesta con su correspondiente tratamiento.</t>
-  </si>
-  <si>
-    <t>HU#9_T1 Creación de los tests correspondientes a las clases que llamen a la API.</t>
-  </si>
-  <si>
-    <t>HU#9_T2 Creación de las clases que realicen llamadas a la API de coinlore.</t>
-  </si>
-  <si>
-    <t>HU#10_T1 Creación de los tests correspondientes a las clases que se encarguen del almacenamiento de los datos en caché.</t>
-  </si>
-  <si>
-    <t>HU#10_T2 Creación de las clases que se encarguen del almacenamiento de los datos en caché.</t>
-  </si>
-  <si>
-    <t>HU#10 Como desarrollador quiero que el proyecto almacene los datos obtenidos de la API en caché.</t>
+    <t>HU#4 Como usuario quiero poder abrir una nueva cartera para poder realizar operaciones con ella.</t>
+  </si>
+  <si>
+    <t>HU#5 Como usuario quiero poder comprar monedas para almacenarlas en la cartera.</t>
+  </si>
+  <si>
+    <t>HU#7 Como usuario quiero consultar un monedero para ver que criptomonedas tiene y su cantidad.</t>
+  </si>
+  <si>
+    <t>HU#8 Como usuario quiero consultar el balance del monedero para obtener información de mi situación financiera.</t>
+  </si>
+  <si>
+    <t>HU#4_T1 Recibir la petición en el archivo routes.</t>
+  </si>
+  <si>
+    <t>HU#4_T2 Validar los parámetros: Etapa Form Request.</t>
+  </si>
+  <si>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t>HU#4_T3 Realizar el controlador de la petición: Etapa Controller</t>
+  </si>
+  <si>
+    <t>HU#4_T4 Realizar la clase servicio de la aplicación: Etapa Service</t>
+  </si>
+  <si>
+    <t>HU#4_T5 Almacenar los datos en la caché: Etapa DataSource</t>
+  </si>
+  <si>
+    <t>HU#4_T6 Realizar petición a la API: API Client</t>
+  </si>
+  <si>
+    <t>HU#5_T1 Recibir la petición en el archivo routes.</t>
+  </si>
+  <si>
+    <t>HU#5_T2 Validar los parámetros: Etapa Form Request.</t>
+  </si>
+  <si>
+    <t>HU#6_T1 Recibir la petición en el archivo routes.</t>
+  </si>
+  <si>
+    <t>HU#6_T2 Validar los parámetros: Etapa Form Request.</t>
+  </si>
+  <si>
+    <t>HU#7_T1 Recibir la petición en el archivo routes.</t>
+  </si>
+  <si>
+    <t>HU#7_T2 Validar los parámetros: Etapa Form Request.</t>
+  </si>
+  <si>
+    <t>HU#7_T3 Realizar el controlador de la petición: Etapa Controller</t>
+  </si>
+  <si>
+    <t>HU#7_T4 Realizar la clase servicio de la aplicación: Etapa Service</t>
+  </si>
+  <si>
+    <t>HU#7_T5 Almacenar los datos en la caché: Etapa DataSource</t>
+  </si>
+  <si>
+    <t>HU#8_T1 Recibir la petición en el archivo routes.</t>
+  </si>
+  <si>
+    <t>HU#8_T2 Validar los parámetros: Etapa Form Request.</t>
+  </si>
+  <si>
+    <t>HU#8_T3 Realizar el controlador de la petición: Etapa Controller</t>
+  </si>
+  <si>
+    <t>HU#8_T4 Realizar la clase servicio de la aplicación: Etapa Service</t>
+  </si>
+  <si>
+    <t>HU#8_T5 Almacenar los datos en la caché: Etapa DataSource</t>
+  </si>
+  <si>
+    <t>HU#6_T3 Realizar el controlador de la petición: Etapa Controller</t>
+  </si>
+  <si>
+    <t>HU#6_T4 Realizar la clase servicio de la aplicación: Etapa Service</t>
+  </si>
+  <si>
+    <t>HU#6_T5 Almacenar los datos en la caché: Etapa DataSource</t>
+  </si>
+  <si>
+    <t>HU#6_T6 Realizar petición a la API: API Client</t>
+  </si>
+  <si>
+    <t>HU#7_T6 Realizar petición a la API: API Client</t>
+  </si>
+  <si>
+    <t>HU#8_T6 Realizar petición a la API: API Client</t>
+  </si>
+  <si>
+    <t>HU#6 Como usuario quiero vender monedas para ganar dinero.</t>
+  </si>
+  <si>
+    <t>HU#5_T3 Realizar el controlador de la petición: Etapa Controller</t>
+  </si>
+  <si>
+    <t>HU#5_T4 Realizar la clase servicio de la aplicación: Etapa Service</t>
+  </si>
+  <si>
+    <t>HU#5_T5 Almacenar los datos en la caché: Etapa DataSource</t>
+  </si>
+  <si>
+    <t>Yeray, Luis</t>
   </si>
 </sst>
 </file>
@@ -327,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -336,7 +396,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,14 +680,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="146.1796875" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="9" max="9" width="43.81640625" customWidth="1"/>
@@ -834,7 +895,9 @@
         <v>40</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -842,7 +905,9 @@
         <v>39</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -867,9 +932,7 @@
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
         <v>29</v>
       </c>
@@ -885,160 +948,333 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="A32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="A35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36" s="1"/>
+      <c r="A36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="B37" s="9"/>
       <c r="C37" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="A38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="B39" s="9"/>
       <c r="C39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="A41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="A42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="B43" s="9"/>
+      <c r="C43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="A44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="8"/>
+      <c r="A47" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" s="9"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="9"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" s="9"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="9"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58" s="9"/>
+      <c r="C58" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58" s="9"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="9"/>
+      <c r="C59" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59" s="9"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61" s="1"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="8"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="8"/>
     </row>
     <row r="88" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>

</xml_diff>

<commit_message>
Documento Historias de Usuario: Modificación 3.0
</commit_message>
<xml_diff>
--- a/Proyecto Final - Historias de Usuario.xlsx
+++ b/Proyecto Final - Historias de Usuario.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Práctica Final Verificación y Validación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEDEA4F-640E-41C4-96B5-CD0D7F08D1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11996859-83CD-45C2-BC05-08D8665ABB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
   <si>
     <t>Julen Huarte Liras</t>
   </si>
@@ -161,58 +161,118 @@
     <t>HU#2_T6 Aplicar pre-commit en el proyecto.</t>
   </si>
   <si>
-    <t>HU#4 Como desarrollador quiero que el proyecto tenga validación de los parámetros de entrada.</t>
-  </si>
-  <si>
-    <t>HU#4_T1 Creación de los tests correspondientes a la etapa REQUEST.</t>
-  </si>
-  <si>
-    <t>HU#4_T2 Creación de las clases correspondientes a la etapa REQUEST con su correspondiente implementación.</t>
-  </si>
-  <si>
-    <t>HU#5 Como Product Owner quiero que el proyecto disponga de controladores para controlar las comunicaciones entre clases de la etapa REQUEST y las de la etapa SERVICE.</t>
-  </si>
-  <si>
-    <t>HU#5_T1 Creación de los tests correspondientes a la etapa CONTROLLER.</t>
-  </si>
-  <si>
-    <t>HU#5_T2 Creación de las clases correspondientes a la etapa CONTROLLER con su correspondiente implementación.</t>
-  </si>
-  <si>
-    <t>HU#6 Como desarrollador quiero que el proyecto tenga unas clases que provean el servicio e implementen la lógica de negocio.</t>
-  </si>
-  <si>
-    <t>HU#6_T1 Creación de los tests correspondientes a la etapa SERVICE.</t>
-  </si>
-  <si>
-    <t>HU#6_T2 Creación de las clases correspondientes a la etapa SERVICE con su correspondiente implementación.</t>
-  </si>
-  <si>
-    <t>HU#7 Como manager del proyecto quiero que el proyecto disponga de unas interfaces que se encarguen de dar respuesta a las peticiones de la etapa SERVICE.</t>
-  </si>
-  <si>
-    <t>HU#8_T1 Creación de los tests correspondientes a la etapa DATASOURCE.</t>
-  </si>
-  <si>
-    <t>HU#8_T2 Creación de las clases correspondientes a la etapa DATASOURCE con su correspondiente implementación.</t>
-  </si>
-  <si>
-    <t>HU#9 Como Product Owner quiero que el proyecto tenga unas clases para que se encarguen de realizar llamadas a la API y recibir su respuesta con su correspondiente tratamiento.</t>
-  </si>
-  <si>
-    <t>HU#9_T1 Creación de los tests correspondientes a las clases que llamen a la API.</t>
-  </si>
-  <si>
-    <t>HU#9_T2 Creación de las clases que realicen llamadas a la API de coinlore.</t>
-  </si>
-  <si>
-    <t>HU#10_T1 Creación de los tests correspondientes a las clases que se encarguen del almacenamiento de los datos en caché.</t>
-  </si>
-  <si>
-    <t>HU#10_T2 Creación de las clases que se encarguen del almacenamiento de los datos en caché.</t>
-  </si>
-  <si>
-    <t>HU#10 Como desarrollador quiero que el proyecto almacene los datos obtenidos de la API en caché.</t>
+    <t>HU#4 Como usuario quiero poder abrir una nueva cartera para poder realizar operaciones con ella.</t>
+  </si>
+  <si>
+    <t>HU#5 Como usuario quiero poder comprar monedas para almacenarlas en la cartera.</t>
+  </si>
+  <si>
+    <t>HU#7 Como usuario quiero consultar un monedero para ver que criptomonedas tiene y su cantidad.</t>
+  </si>
+  <si>
+    <t>HU#8 Como usuario quiero consultar el balance del monedero para obtener información de mi situación financiera.</t>
+  </si>
+  <si>
+    <t>HU#4_T1 Recibir la petición en el archivo routes.</t>
+  </si>
+  <si>
+    <t>HU#4_T2 Validar los parámetros: Etapa Form Request.</t>
+  </si>
+  <si>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t>HU#4_T3 Realizar el controlador de la petición: Etapa Controller</t>
+  </si>
+  <si>
+    <t>HU#4_T4 Realizar la clase servicio de la aplicación: Etapa Service</t>
+  </si>
+  <si>
+    <t>HU#4_T5 Almacenar los datos en la caché: Etapa DataSource</t>
+  </si>
+  <si>
+    <t>HU#4_T6 Realizar petición a la API: API Client</t>
+  </si>
+  <si>
+    <t>HU#5_T1 Recibir la petición en el archivo routes.</t>
+  </si>
+  <si>
+    <t>HU#5_T2 Validar los parámetros: Etapa Form Request.</t>
+  </si>
+  <si>
+    <t>HU#6_T1 Recibir la petición en el archivo routes.</t>
+  </si>
+  <si>
+    <t>HU#6_T2 Validar los parámetros: Etapa Form Request.</t>
+  </si>
+  <si>
+    <t>HU#7_T1 Recibir la petición en el archivo routes.</t>
+  </si>
+  <si>
+    <t>HU#7_T2 Validar los parámetros: Etapa Form Request.</t>
+  </si>
+  <si>
+    <t>HU#7_T3 Realizar el controlador de la petición: Etapa Controller</t>
+  </si>
+  <si>
+    <t>HU#7_T4 Realizar la clase servicio de la aplicación: Etapa Service</t>
+  </si>
+  <si>
+    <t>HU#7_T5 Almacenar los datos en la caché: Etapa DataSource</t>
+  </si>
+  <si>
+    <t>HU#8_T1 Recibir la petición en el archivo routes.</t>
+  </si>
+  <si>
+    <t>HU#8_T2 Validar los parámetros: Etapa Form Request.</t>
+  </si>
+  <si>
+    <t>HU#8_T3 Realizar el controlador de la petición: Etapa Controller</t>
+  </si>
+  <si>
+    <t>HU#8_T4 Realizar la clase servicio de la aplicación: Etapa Service</t>
+  </si>
+  <si>
+    <t>HU#8_T5 Almacenar los datos en la caché: Etapa DataSource</t>
+  </si>
+  <si>
+    <t>HU#6_T3 Realizar el controlador de la petición: Etapa Controller</t>
+  </si>
+  <si>
+    <t>HU#6_T4 Realizar la clase servicio de la aplicación: Etapa Service</t>
+  </si>
+  <si>
+    <t>HU#6_T5 Almacenar los datos en la caché: Etapa DataSource</t>
+  </si>
+  <si>
+    <t>HU#6_T6 Realizar petición a la API: API Client</t>
+  </si>
+  <si>
+    <t>HU#7_T6 Realizar petición a la API: API Client</t>
+  </si>
+  <si>
+    <t>HU#8_T6 Realizar petición a la API: API Client</t>
+  </si>
+  <si>
+    <t>HU#6 Como usuario quiero vender monedas para ganar dinero.</t>
+  </si>
+  <si>
+    <t>HU#5_T3 Realizar el controlador de la petición: Etapa Controller</t>
+  </si>
+  <si>
+    <t>HU#5_T4 Realizar la clase servicio de la aplicación: Etapa Service</t>
+  </si>
+  <si>
+    <t>HU#5_T5 Almacenar los datos en la caché: Etapa DataSource</t>
+  </si>
+  <si>
+    <t>Yeray, Luis</t>
   </si>
 </sst>
 </file>
@@ -327,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -336,7 +396,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,14 +680,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="146.1796875" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="9" max="9" width="43.81640625" customWidth="1"/>
@@ -834,7 +895,9 @@
         <v>40</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -842,7 +905,9 @@
         <v>39</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -867,9 +932,7 @@
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
         <v>29</v>
       </c>
@@ -885,160 +948,333 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="A32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="A35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36" s="1"/>
+      <c r="A36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="B37" s="9"/>
       <c r="C37" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="A38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="B39" s="9"/>
       <c r="C39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="A41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="A42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="B43" s="9"/>
+      <c r="C43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="A44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="8"/>
+      <c r="A47" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" s="9"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="9"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" s="9"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="9"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58" s="9"/>
+      <c r="C58" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58" s="9"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="9"/>
+      <c r="C59" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59" s="9"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61" s="1"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="8"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="8"/>
     </row>
     <row r="88" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>

</xml_diff>

<commit_message>
Documento Historias de Usuario modificado y proyecto finalizado
</commit_message>
<xml_diff>
--- a/Proyecto Final - Historias de Usuario.xlsx
+++ b/Proyecto Final - Historias de Usuario.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\verificacion_y_validacion\proyecto-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11996859-83CD-45C2-BC05-08D8665ABB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61345B3-6DC7-492B-9FCC-B0570B19A947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Julen Huarte Liras</t>
   </si>
@@ -47,21 +47,9 @@
     <t>Historias de Usuario</t>
   </si>
   <si>
-    <t>Responsable</t>
-  </si>
-  <si>
-    <t>Estimado</t>
-  </si>
-  <si>
-    <t>Realizado</t>
-  </si>
-  <si>
     <t>HU#1_T2 Estimar duración de las tareas.</t>
   </si>
   <si>
-    <t>Julen</t>
-  </si>
-  <si>
     <t>Yeray Aller Errea</t>
   </si>
   <si>
@@ -110,42 +98,6 @@
     <t>HU#2 Como manager del proyecto quiero configurar un entorno de trabajo para desempeñar correctamente las tareas del desarrollo del proyecto.</t>
   </si>
   <si>
-    <t>Julen, Yeray, Luis, Javi</t>
-  </si>
-  <si>
-    <t>Yeray</t>
-  </si>
-  <si>
-    <t>Yeray, Luis, Javi</t>
-  </si>
-  <si>
-    <t>1h</t>
-  </si>
-  <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>3h</t>
-  </si>
-  <si>
-    <t>15min</t>
-  </si>
-  <si>
-    <t>25min</t>
-  </si>
-  <si>
-    <t>10min</t>
-  </si>
-  <si>
-    <t>30min</t>
-  </si>
-  <si>
-    <t>45min</t>
-  </si>
-  <si>
-    <t>1h 30min</t>
-  </si>
-  <si>
     <t>HU#3_T1 Creación de los tests correspondientes a las clases de modelo.</t>
   </si>
   <si>
@@ -179,15 +131,6 @@
     <t>HU#4_T2 Validar los parámetros: Etapa Form Request.</t>
   </si>
   <si>
-    <t>5 min</t>
-  </si>
-  <si>
-    <t>4h</t>
-  </si>
-  <si>
-    <t>6h</t>
-  </si>
-  <si>
     <t>HU#4_T3 Realizar el controlador de la petición: Etapa Controller</t>
   </si>
   <si>
@@ -270,9 +213,6 @@
   </si>
   <si>
     <t>HU#5_T5 Almacenar los datos en la caché: Etapa DataSource</t>
-  </si>
-  <si>
-    <t>Yeray, Luis</t>
   </si>
 </sst>
 </file>
@@ -349,7 +289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -376,9 +316,20 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </right>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -387,17 +338,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,7 +633,7 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -695,47 +647,47 @@
   <sheetData>
     <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -746,535 +698,425 @@
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="9"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D39" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D45" s="9"/>
+        <v>49</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D50" s="9"/>
+        <v>39</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D51" s="9"/>
+        <v>40</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D52" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D53" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D54" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D55" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D57" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D58" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D59" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D60" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D61" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D62" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="8"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" s="8"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="7"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="10"/>
+      <c r="B66" s="7"/>
     </row>
     <row r="88" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>

</xml_diff>

<commit_message>
Documento de Historias Actualizado con las tareas de la nueva iteración
</commit_message>
<xml_diff>
--- a/Proyecto Final - Historias de Usuario.xlsx
+++ b/Proyecto Final - Historias de Usuario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\verificacion_y_validacion\proyecto-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61345B3-6DC7-492B-9FCC-B0570B19A947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940445B0-BB89-481D-A2D3-D9EEAFFD98A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Julen Huarte Liras</t>
   </si>
@@ -213,6 +213,18 @@
   </si>
   <si>
     <t>HU#5_T5 Almacenar los datos en la caché: Etapa DataSource</t>
+  </si>
+  <si>
+    <t>HU#9_T3 Implementar Integración Continua</t>
+  </si>
+  <si>
+    <t>HU#9_T1 Arreglar tests erroneos.</t>
+  </si>
+  <si>
+    <t>HU#9_T2 Implementar tests que faltaban.</t>
+  </si>
+  <si>
+    <t>HU#9 Como manager del proyecto quiero solucionar los errores provenientes de la iteración anterior.</t>
   </si>
 </sst>
 </file>
@@ -289,7 +301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -312,44 +324,19 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,478 +632,322 @@
     <col min="9" max="9" width="43.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-    </row>
-    <row r="43" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="10"/>
-      <c r="B63" s="7"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" s="10"/>
-      <c r="B66" s="7"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="88" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>

</xml_diff>